<commit_message>
update work after back to China
</commit_message>
<xml_diff>
--- a/doc/experiment_plan.xlsx
+++ b/doc/experiment_plan.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20349"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4080E24A-B54E-436C-9555-9F481C3E0E65}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C28FD90-7917-4C07-9B3C-7739F1FD6C60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mini5_experiment" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>LSTM</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -214,6 +214,10 @@
   </si>
   <si>
     <t>Not good. 98.96 accuracy. 21.5hr training, Slow convergence.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bad. Less than 70%, No test.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -325,9 +329,6 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -335,6 +336,9 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -617,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -634,14 +638,14 @@
       <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -655,19 +659,19 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -681,24 +685,24 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.6">
-      <c r="A5" s="2"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="2"/>
+      <c r="A7" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -717,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E612C8F-7766-40B1-A4DE-073CC66575C0}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -738,22 +742,22 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2"/>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A3" s="2"/>
+      <c r="A3" s="9"/>
       <c r="B3" t="s">
         <v>23</v>
       </c>
@@ -774,36 +778,39 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="16.5" x14ac:dyDescent="0.6">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="G5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A6" s="2"/>
+      <c r="A6" s="9"/>
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -821,25 +828,25 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="16.5" x14ac:dyDescent="0.6">
-      <c r="A7" s="2"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G8" t="s">
@@ -850,10 +857,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A9" s="2"/>
+      <c r="A9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A10" s="2"/>
+      <c r="A10" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -883,11 +890,11 @@
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">

</xml_diff>